<commit_message>
changed datatype some variables
</commit_message>
<xml_diff>
--- a/localidades_limpio.xlsx
+++ b/localidades_limpio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RYZEN 5\Downloads\Proyecto MLDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E90DBB5-8ACC-4BE3-8784-9961EC643926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B580587-867A-48AA-AFFA-648D666A5813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="690" windowWidth="11490" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,11 +288,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,14 +599,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98:B103"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -611,22 +619,22 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -636,29 +644,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>4569</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>77979</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>9.5</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>1513</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>111.34</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>2.9</v>
       </c>
       <c r="I2" t="s">
@@ -668,29 +676,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>4569</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>77073</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>9.5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>1540</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>109.71</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>2.9</v>
       </c>
       <c r="I3" t="s">
@@ -700,29 +708,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>4569</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>76222</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>9.5</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>1415</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>108.7</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>2.9</v>
       </c>
       <c r="I4" t="s">
@@ -732,29 +740,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>4569</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>75425</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>9.5</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>1452</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>101.3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>2.9</v>
       </c>
       <c r="I5" t="s">
@@ -764,29 +772,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>4569</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>74526</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>9.5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>1504</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>100.1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>2.9</v>
       </c>
       <c r="I6" t="s">
@@ -796,29 +804,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>4569</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>73556</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>9.5</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1617</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>113.3</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>2.9</v>
       </c>
       <c r="I7" t="s">
@@ -828,29 +836,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2010</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>62</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>15707</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>416</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>121.3</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>2.6</v>
       </c>
       <c r="I8" t="s">
@@ -860,29 +868,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>62</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>15621</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>7</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>445</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>113.58</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>2.6</v>
       </c>
       <c r="I9" t="s">
@@ -892,29 +900,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2012</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>62</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>15477</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>7</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>461</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>106.8</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>2.6</v>
       </c>
       <c r="I10" t="s">
@@ -924,29 +932,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2013</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>62</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>15297</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>7</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>510</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>98.6</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>2.6</v>
       </c>
       <c r="I11" t="s">
@@ -956,29 +964,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2014</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>62</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>14982</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>7</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>528</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>97.4</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>2.6</v>
       </c>
       <c r="I12" t="s">
@@ -988,29 +996,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2015</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>62</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>14525</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>7</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>607</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>102.9</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>2.6</v>
       </c>
       <c r="I13" t="s">
@@ -1020,29 +1028,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>1665</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>22008</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>22.5</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>405</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>94.9</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>6.3</v>
       </c>
       <c r="I14" t="s">
@@ -1052,29 +1060,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>1665</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>21521</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>22.5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>424</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>88.74</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>6.3</v>
       </c>
       <c r="I15" t="s">
@@ -1084,29 +1092,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>1665</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>21068</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>22.5</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>437</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>85.6</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>6.3</v>
       </c>
       <c r="I16" t="s">
@@ -1116,29 +1124,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2013</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>1665</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>20650</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>22.5</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>452</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>82.9</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>6.3</v>
       </c>
       <c r="I17" t="s">
@@ -1148,29 +1156,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2014</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>1665</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>20267</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>22.5</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>481</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>78.2</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>6.3</v>
       </c>
       <c r="I18" t="s">
@@ -1180,29 +1188,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2015</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>1665</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>19933</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>22.5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>500</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>79.5</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>6.3</v>
       </c>
       <c r="I19" t="s">
@@ -1212,29 +1220,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2010</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>2615</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>94043</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>26.5</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>347</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>99.94</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
         <v>4.8</v>
       </c>
       <c r="I20" t="s">
@@ -1244,29 +1252,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>2615</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>91938</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>26.5</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>393</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>98.85</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>4.8</v>
       </c>
       <c r="I21" t="s">
@@ -1276,29 +1284,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2012</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>2615</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>90009</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>26.5</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>472</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>95.1</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>4.8</v>
       </c>
       <c r="I22" t="s">
@@ -1308,29 +1316,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2013</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>2615</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>88212</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>26.5</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>500</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>93.6</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>4.8</v>
       </c>
       <c r="I23" t="s">
@@ -1340,29 +1348,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2014</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>2615</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>86662</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>26.5</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>511</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>95.5</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>4.8</v>
       </c>
       <c r="I24" t="s">
@@ -1372,29 +1380,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2015</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>2615</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>85160</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>26.5</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>846</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>93.4</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="3">
         <v>4.8</v>
       </c>
       <c r="I25" t="s">
@@ -1404,29 +1412,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2010</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>13128</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>92612</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>31.5</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>1498</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>96.79</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I26" t="s">
@@ -1436,29 +1444,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2011</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>13128</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="3">
         <v>95305</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3">
         <v>31.5</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>1600</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>91.24</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I27" t="s">
@@ -1468,29 +1476,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2012</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>13128</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <v>97700</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3">
         <v>31.5</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>1635</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>85.2</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I28" t="s">
@@ -1500,29 +1508,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2013</v>
       </c>
       <c r="B29" t="s">
         <v>22</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>13128</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <v>99646</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3">
         <v>31.5</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>1744</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>84.5</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I29" t="s">
@@ -1532,29 +1540,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2014</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>13128</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="3">
         <v>101152</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3">
         <v>31.5</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <v>1871</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="3">
         <v>83.2</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I30" t="s">
@@ -1564,29 +1572,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2015</v>
       </c>
       <c r="B31" t="s">
         <v>22</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>13128</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="3">
         <v>101784</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <v>31.5</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>1982</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="3">
         <v>78.7</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I31" t="s">
@@ -1596,29 +1604,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2010</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
         <v>41970</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3">
         <v>17.5</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <v>38</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="3">
         <v>149.4</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>3.6</v>
       </c>
       <c r="I32" t="s">
@@ -1628,29 +1636,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
         <v>41074</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="3">
         <v>17.5</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="3">
         <v>38</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="3">
         <v>149.28</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="3">
         <v>3.6</v>
       </c>
       <c r="I33" t="s">
@@ -1660,29 +1668,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2012</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
         <v>40207</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="3">
         <v>17.5</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>46</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="3">
         <v>145.19999999999999</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="3">
         <v>3.6</v>
       </c>
       <c r="I34" t="s">
@@ -1692,29 +1700,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2013</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
         <v>39422</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="3">
         <v>17.5</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <v>48</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="3">
         <v>147.5</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="3">
         <v>3.6</v>
       </c>
       <c r="I35" t="s">
@@ -1724,29 +1732,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2014</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
         <v>38637</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="3">
         <v>17.5</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>48</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="3">
         <v>147.30000000000001</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="3">
         <v>3.6</v>
       </c>
       <c r="I36" t="s">
@@ -1756,29 +1764,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2015</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
         <v>37833</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="3">
         <v>17.5</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="3">
         <v>48</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="3">
         <v>144.80000000000001</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="3">
         <v>3.6</v>
       </c>
       <c r="I37" t="s">
@@ -1788,29 +1796,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2010</v>
       </c>
       <c r="B38" t="s">
         <v>28</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3">
         <v>17162</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="3">
         <v>135188</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="3">
         <v>24.5</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="3">
         <v>1019</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="3">
         <v>108.15</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="3">
         <v>5.2</v>
       </c>
       <c r="I38" t="s">
@@ -1820,29 +1828,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2011</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>17162</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="3">
         <v>135780</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="3">
         <v>24.5</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="3">
         <v>1172</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="3">
         <v>107.05</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="3">
         <v>5.2</v>
       </c>
       <c r="I39" t="s">
@@ -1852,29 +1860,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2012</v>
       </c>
       <c r="B40" t="s">
         <v>28</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <v>17162</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="3">
         <v>136572</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="3">
         <v>24.5</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="3">
         <v>1395</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="3">
         <v>104.1</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="3">
         <v>5.2</v>
       </c>
       <c r="I40" t="s">
@@ -1884,29 +1892,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2013</v>
       </c>
       <c r="B41" t="s">
         <v>28</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3">
         <v>17162</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="3">
         <v>137696</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="3">
         <v>24.5</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <v>1783</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="3">
         <v>108.2</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="3">
         <v>5.2</v>
       </c>
       <c r="I41" t="s">
@@ -1916,29 +1924,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2014</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="3">
         <v>17162</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="3">
         <v>139262</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="3">
         <v>24.5</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="3">
         <v>2006</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="3">
         <v>107.7</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="3">
         <v>5.2</v>
       </c>
       <c r="I42" t="s">
@@ -1948,29 +1956,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2015</v>
       </c>
       <c r="B43" t="s">
         <v>28</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="3">
         <v>17162</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="3">
         <v>141463</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="3">
         <v>24.5</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>2195</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>104</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="3">
         <v>5.2</v>
       </c>
       <c r="I43" t="s">
@@ -1980,29 +1988,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2010</v>
       </c>
       <c r="B44" t="s">
         <v>31</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="3">
         <v>2718</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="3">
         <v>206938</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="3">
         <v>15</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="3">
         <v>638</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="3">
         <v>88.41</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="3">
         <v>4</v>
       </c>
       <c r="I44" t="s">
@@ -2012,29 +2020,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2011</v>
       </c>
       <c r="B45" t="s">
         <v>31</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="3">
         <v>2718</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="3">
         <v>205083</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="3">
         <v>15</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <v>620</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="3">
         <v>90.82</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="3">
         <v>4</v>
       </c>
       <c r="I45" t="s">
@@ -2044,29 +2052,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2012</v>
       </c>
       <c r="B46" t="s">
         <v>31</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="3">
         <v>2718</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="3">
         <v>203545</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="3">
         <v>15</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <v>549</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="3">
         <v>89.7</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="3">
         <v>4</v>
       </c>
       <c r="I46" t="s">
@@ -2076,29 +2084,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2013</v>
       </c>
       <c r="B47" t="s">
         <v>31</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="3">
         <v>2718</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="3">
         <v>202186</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="3">
         <v>15</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>748</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="3">
         <v>88.1</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="3">
         <v>4</v>
       </c>
       <c r="I47" t="s">
@@ -2108,29 +2116,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2014</v>
       </c>
       <c r="B48" t="s">
         <v>31</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="3">
         <v>2718</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="3">
         <v>200994</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="3">
         <v>15</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>834</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="3">
         <v>88.3</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="3">
         <v>4</v>
       </c>
       <c r="I48" t="s">
@@ -2140,29 +2148,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2015</v>
       </c>
       <c r="B49" t="s">
         <v>31</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="3">
         <v>2718</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="3">
         <v>200086</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="3">
         <v>15</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>1015</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>88.3</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="3">
         <v>4</v>
       </c>
       <c r="I49" t="s">
@@ -2172,29 +2180,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2010</v>
       </c>
       <c r="B50" t="s">
         <v>34</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="3">
         <v>17400</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="3">
         <v>64300</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="3">
         <v>9</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <v>123</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="3">
         <v>86.72</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="I50" t="s">
@@ -2204,29 +2212,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2011</v>
       </c>
       <c r="B51" t="s">
         <v>34</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="3">
         <v>17400</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="3">
         <v>64394</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="3">
         <v>9</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <v>119</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="3">
         <v>84.84</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="I51" t="s">
@@ -2236,29 +2244,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2012</v>
       </c>
       <c r="B52" t="s">
         <v>34</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="3">
         <v>17400</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="3">
         <v>64563</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="3">
         <v>9</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <v>119</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="3">
         <v>82.8</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="I52" t="s">
@@ -2268,29 +2276,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2013</v>
       </c>
       <c r="B53" t="s">
         <v>34</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="3">
         <v>17400</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="3">
         <v>64811</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="3">
         <v>9</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>119</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="3">
         <v>81.5</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="I53" t="s">
@@ -2300,29 +2308,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2014</v>
       </c>
       <c r="B54" t="s">
         <v>34</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="3">
         <v>17400</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="3">
         <v>65172</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="3">
         <v>9</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>119</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="3">
         <v>78.599999999999994</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="I54" t="s">
@@ -2332,29 +2340,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2015</v>
       </c>
       <c r="B55" t="s">
         <v>34</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="3">
         <v>17400</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="3">
         <v>65692</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="3">
         <v>9</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <v>119</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="3">
         <v>80.3</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="I55" t="s">
@@ -2364,29 +2372,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2010</v>
       </c>
       <c r="B56" t="s">
         <v>37</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="3">
         <v>1740</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="3">
         <v>153243</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="3">
         <v>9</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <v>323</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="3">
         <v>102.97</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="3">
         <v>5.4</v>
       </c>
       <c r="I56" t="s">
@@ -2396,29 +2404,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2011</v>
       </c>
       <c r="B57" t="s">
         <v>37</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="3">
         <v>1740</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="3">
         <v>151462</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="3">
         <v>9</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="3">
         <v>311</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="3">
         <v>98.76</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="3">
         <v>5.4</v>
       </c>
       <c r="I57" t="s">
@@ -2428,29 +2436,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2012</v>
       </c>
       <c r="B58" t="s">
         <v>37</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="3">
         <v>1740</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="3">
         <v>149694</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="3">
         <v>9</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <v>56</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="3">
         <v>96.4</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="3">
         <v>5.4</v>
       </c>
       <c r="I58" t="s">
@@ -2460,29 +2468,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2013</v>
       </c>
       <c r="B59" t="s">
         <v>37</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="3">
         <v>1740</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="3">
         <v>147957</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="3">
         <v>9</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="3">
         <v>60</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="3">
         <v>95.4</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="3">
         <v>5.4</v>
       </c>
       <c r="I59" t="s">
@@ -2492,29 +2500,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2014</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="3">
         <v>1740</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="3">
         <v>146283</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="3">
         <v>9</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <v>63</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="3">
         <v>97.8</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="3">
         <v>5.4</v>
       </c>
       <c r="I60" t="s">
@@ -2524,29 +2532,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2015</v>
       </c>
       <c r="B61" t="s">
         <v>37</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="3">
         <v>1740</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="3">
         <v>144910</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="3">
         <v>9</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="3">
         <v>63</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="3">
         <v>95.7</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="3">
         <v>5.4</v>
       </c>
       <c r="I61" t="s">
@@ -2556,29 +2564,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2010</v>
       </c>
       <c r="B62" t="s">
         <v>40</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="3">
         <v>160</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="3">
         <v>205546</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="3">
         <v>10</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="3">
         <v>647</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="3">
         <v>106.17</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="3">
         <v>3.9</v>
       </c>
       <c r="I62" t="s">
@@ -2588,29 +2596,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2011</v>
       </c>
       <c r="B63" t="s">
         <v>40</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="3">
         <v>160</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="3">
         <v>206024</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="3">
         <v>10</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="3">
         <v>670</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="3">
         <v>101.71</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="3">
         <v>3.9</v>
       </c>
       <c r="I63" t="s">
@@ -2620,29 +2628,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2012</v>
       </c>
       <c r="B64" t="s">
         <v>40</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="3">
         <v>160</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="3">
         <v>206813</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="3">
         <v>10</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="3">
         <v>677</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="3">
         <v>100.3</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="3">
         <v>3.9</v>
       </c>
       <c r="I64" t="s">
@@ -2652,29 +2660,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2013</v>
       </c>
       <c r="B65" t="s">
         <v>40</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="3">
         <v>160</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="3">
         <v>207803</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="3">
         <v>10</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="3">
         <v>745</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="3">
         <v>99.6</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="3">
         <v>3.9</v>
       </c>
       <c r="I65" t="s">
@@ -2684,29 +2692,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2014</v>
       </c>
       <c r="B66" t="s">
         <v>40</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="3">
         <v>160</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="3">
         <v>209010</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="3">
         <v>10</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="3">
         <v>800</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="3">
         <v>98.1</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="3">
         <v>3.9</v>
       </c>
       <c r="I66" t="s">
@@ -2716,29 +2724,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2015</v>
       </c>
       <c r="B67" t="s">
         <v>40</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="3">
         <v>160</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="3">
         <v>210420</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="3">
         <v>10</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="3">
         <v>778</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="3">
         <v>96.5</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="3">
         <v>3.9</v>
       </c>
       <c r="I67" t="s">
@@ -2748,29 +2756,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2010</v>
       </c>
       <c r="B68" t="s">
         <v>43</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="3">
         <v>834</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="3">
         <v>35453</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="3">
         <v>10</v>
       </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3">
         <v>87.49</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="3">
         <v>3</v>
       </c>
       <c r="I68" t="s">
@@ -2780,29 +2788,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2011</v>
       </c>
       <c r="B69" t="s">
         <v>43</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="3">
         <v>834</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="3">
         <v>34884</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="3">
         <v>10</v>
       </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
+      <c r="F69" s="3">
+        <v>0</v>
+      </c>
+      <c r="G69" s="3">
         <v>82.76</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="3">
         <v>3</v>
       </c>
       <c r="I69" t="s">
@@ -2812,29 +2820,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2012</v>
       </c>
       <c r="B70" t="s">
         <v>43</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="3">
         <v>834</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="3">
         <v>34288</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="3">
         <v>10</v>
       </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
+      <c r="F70" s="3">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3">
         <v>80.400000000000006</v>
       </c>
-      <c r="H70">
+      <c r="H70" s="3">
         <v>3</v>
       </c>
       <c r="I70" t="s">
@@ -2844,29 +2852,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2013</v>
       </c>
       <c r="B71" t="s">
         <v>43</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="3">
         <v>834</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="3">
         <v>33730</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="3">
         <v>10</v>
       </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
+      <c r="F71" s="3">
+        <v>0</v>
+      </c>
+      <c r="G71" s="3">
         <v>78.2</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="3">
         <v>3</v>
       </c>
       <c r="I71" t="s">
@@ -2876,29 +2884,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2014</v>
       </c>
       <c r="B72" t="s">
         <v>43</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="3">
         <v>834</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="3">
         <v>33123</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="3">
         <v>10</v>
       </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
+      <c r="F72" s="3">
+        <v>0</v>
+      </c>
+      <c r="G72" s="3">
         <v>80.5</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="3">
         <v>3</v>
       </c>
       <c r="I72" t="s">
@@ -2908,29 +2916,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2015</v>
       </c>
       <c r="B73" t="s">
         <v>43</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="3">
         <v>834</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="3">
         <v>32633</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="3">
         <v>10</v>
       </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
+      <c r="F73" s="3">
+        <v>0</v>
+      </c>
+      <c r="G73" s="3">
         <v>75.5</v>
       </c>
-      <c r="H73">
+      <c r="H73" s="3">
         <v>3</v>
       </c>
       <c r="I73" t="s">
@@ -2940,29 +2948,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2010</v>
       </c>
       <c r="B74" t="s">
         <v>46</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="3">
         <v>140</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="3">
         <v>17913</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="3">
         <v>4</v>
       </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74">
+      <c r="F74" s="3">
+        <v>0</v>
+      </c>
+      <c r="G74" s="3">
         <v>126.23</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="3">
         <v>4.2</v>
       </c>
       <c r="I74" t="s">
@@ -2972,29 +2980,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2011</v>
       </c>
       <c r="B75" t="s">
         <v>46</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="3">
         <v>140</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="3">
         <v>17731</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="3">
         <v>4</v>
       </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-      <c r="G75">
+      <c r="F75" s="3">
+        <v>0</v>
+      </c>
+      <c r="G75" s="3">
         <v>133.59</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="3">
         <v>4.2</v>
       </c>
       <c r="I75" t="s">
@@ -3004,29 +3012,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2012</v>
       </c>
       <c r="B76" t="s">
         <v>46</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="3">
         <v>140</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="3">
         <v>17506</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="3">
         <v>4</v>
       </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-      <c r="G76">
+      <c r="F76" s="3">
+        <v>0</v>
+      </c>
+      <c r="G76" s="3">
         <v>129.1</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="3">
         <v>4.2</v>
       </c>
       <c r="I76" t="s">
@@ -3036,29 +3044,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2013</v>
       </c>
       <c r="B77" t="s">
         <v>46</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="3">
         <v>140</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="3">
         <v>17271</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="3">
         <v>4</v>
       </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
+      <c r="F77" s="3">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3">
         <v>120.6</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="3">
         <v>4.2</v>
       </c>
       <c r="I77" t="s">
@@ -3068,29 +3076,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2014</v>
       </c>
       <c r="B78" t="s">
         <v>46</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="3">
         <v>140</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="3">
         <v>16933</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="3">
         <v>4</v>
       </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
+      <c r="F78" s="3">
+        <v>0</v>
+      </c>
+      <c r="G78" s="3">
         <v>127</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="3">
         <v>4.2</v>
       </c>
       <c r="I78" t="s">
@@ -3100,29 +3108,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2015</v>
       </c>
       <c r="B79" t="s">
         <v>46</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="3">
         <v>140</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="3">
         <v>16501</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="3">
         <v>4</v>
       </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
+      <c r="F79" s="3">
+        <v>0</v>
+      </c>
+      <c r="G79" s="3">
         <v>133.30000000000001</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="3">
         <v>4.2</v>
       </c>
       <c r="I79" t="s">
@@ -3132,29 +3140,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2010</v>
       </c>
       <c r="B80" t="s">
         <v>49</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="3">
         <v>1800</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="3">
         <v>16508</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="3">
         <v>18</v>
       </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
+      <c r="F80" s="3">
+        <v>0</v>
+      </c>
+      <c r="G80" s="3">
         <v>146.65</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="3">
         <v>4.7</v>
       </c>
       <c r="I80" t="s">
@@ -3164,29 +3172,29 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2011</v>
       </c>
       <c r="B81" t="s">
         <v>49</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="3">
         <v>1800</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="3">
         <v>16262</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="3">
         <v>18</v>
       </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-      <c r="G81">
+      <c r="F81" s="3">
+        <v>0</v>
+      </c>
+      <c r="G81" s="3">
         <v>145.31</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="3">
         <v>4.7</v>
       </c>
       <c r="I81" t="s">
@@ -3196,29 +3204,29 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2012</v>
       </c>
       <c r="B82" t="s">
         <v>49</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="3">
         <v>1800</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="3">
         <v>15993</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="3">
         <v>18</v>
       </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-      <c r="G82">
+      <c r="F82" s="3">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3">
         <v>143.80000000000001</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="3">
         <v>4.7</v>
       </c>
       <c r="I82" t="s">
@@ -3228,29 +3236,29 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2013</v>
       </c>
       <c r="B83" t="s">
         <v>49</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="3">
         <v>1800</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="3">
         <v>15702</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="3">
         <v>18</v>
       </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-      <c r="G83">
+      <c r="F83" s="3">
+        <v>0</v>
+      </c>
+      <c r="G83" s="3">
         <v>136.1</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="3">
         <v>4.7</v>
       </c>
       <c r="I83" t="s">
@@ -3260,29 +3268,29 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2014</v>
       </c>
       <c r="B84" t="s">
         <v>49</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="3">
         <v>1800</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="3">
         <v>15385</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="3">
         <v>18</v>
       </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84">
+      <c r="F84" s="3">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3">
         <v>134.6</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="3">
         <v>4.7</v>
       </c>
       <c r="I84" t="s">
@@ -3292,29 +3300,29 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2015</v>
       </c>
       <c r="B85" t="s">
         <v>49</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="3">
         <v>1800</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="3">
         <v>15011</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="3">
         <v>18</v>
       </c>
-      <c r="F85">
-        <v>0</v>
-      </c>
-      <c r="G85">
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
+      <c r="G85" s="3">
         <v>134.69999999999999</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="3">
         <v>4.7</v>
       </c>
       <c r="I85" t="s">
@@ -3324,29 +3332,29 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2010</v>
       </c>
       <c r="B86" t="s">
         <v>52</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="3">
         <v>93</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="3">
         <v>20881</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="3">
         <v>12</v>
       </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-      <c r="G86">
+      <c r="F86" s="3">
+        <v>0</v>
+      </c>
+      <c r="G86" s="3">
         <v>123.43</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="3">
         <v>3.4</v>
       </c>
       <c r="I86" t="s">
@@ -3356,29 +3364,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2011</v>
       </c>
       <c r="B87" t="s">
         <v>52</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="3">
         <v>93</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="3">
         <v>20473</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="3">
         <v>12</v>
       </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
-      <c r="G87">
+      <c r="F87" s="3">
+        <v>0</v>
+      </c>
+      <c r="G87" s="3">
         <v>125.47</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="3">
         <v>3.4</v>
       </c>
       <c r="I87" t="s">
@@ -3388,29 +3396,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2012</v>
       </c>
       <c r="B88" t="s">
         <v>52</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="3">
         <v>93</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="3">
         <v>20096</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="3">
         <v>12</v>
       </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-      <c r="G88">
+      <c r="F88" s="3">
+        <v>0</v>
+      </c>
+      <c r="G88" s="3">
         <v>118.8</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="3">
         <v>3.4</v>
       </c>
       <c r="I88" t="s">
@@ -3420,29 +3428,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2013</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="3">
         <v>93</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="3">
         <v>19727</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="3">
         <v>12</v>
       </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-      <c r="G89">
+      <c r="F89" s="3">
+        <v>0</v>
+      </c>
+      <c r="G89" s="3">
         <v>113.1</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="3">
         <v>3.4</v>
       </c>
       <c r="I89" t="s">
@@ -3452,29 +3460,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2014</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="3">
         <v>93</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="3">
         <v>19360</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="3">
         <v>12</v>
       </c>
-      <c r="F90">
-        <v>0</v>
-      </c>
-      <c r="G90">
+      <c r="F90" s="3">
+        <v>0</v>
+      </c>
+      <c r="G90" s="3">
         <v>120.2</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="3">
         <v>3.4</v>
       </c>
       <c r="I90" t="s">
@@ -3484,29 +3492,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2015</v>
       </c>
       <c r="B91" t="s">
         <v>52</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="3">
         <v>93</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="3">
         <v>18977</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="3">
         <v>12</v>
       </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
-      <c r="G91">
+      <c r="F91" s="3">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3">
         <v>116.8</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="3">
         <v>3.4</v>
       </c>
       <c r="I91" t="s">
@@ -3516,29 +3524,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2010</v>
       </c>
       <c r="B92" t="s">
         <v>55</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="3">
         <v>3352</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="3">
         <v>44630</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="3">
         <v>11.5</v>
       </c>
-      <c r="F92">
-        <v>0</v>
-      </c>
-      <c r="G92">
+      <c r="F92" s="3">
+        <v>0</v>
+      </c>
+      <c r="G92" s="3">
         <v>112.45</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="3">
         <v>4.5</v>
       </c>
       <c r="I92" t="s">
@@ -3548,29 +3556,29 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2011</v>
       </c>
       <c r="B93" t="s">
         <v>55</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="3">
         <v>3352</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="3">
         <v>43590</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="3">
         <v>11.5</v>
       </c>
-      <c r="F93">
-        <v>0</v>
-      </c>
-      <c r="G93">
+      <c r="F93" s="3">
+        <v>0</v>
+      </c>
+      <c r="G93" s="3">
         <v>113.96</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="3">
         <v>4.5</v>
       </c>
       <c r="I93" t="s">
@@ -3580,29 +3588,29 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2012</v>
       </c>
       <c r="B94" t="s">
         <v>55</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="3">
         <v>3352</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="3">
         <v>42599</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="3">
         <v>11.5</v>
       </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-      <c r="G94">
+      <c r="F94" s="3">
+        <v>0</v>
+      </c>
+      <c r="G94" s="3">
         <v>110.8</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="3">
         <v>4.5</v>
       </c>
       <c r="I94" t="s">
@@ -3612,29 +3620,29 @@
         <v>57</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2013</v>
       </c>
       <c r="B95" t="s">
         <v>55</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="3">
         <v>3352</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="3">
         <v>41672</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="3">
         <v>11.5</v>
       </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
-      <c r="G95">
+      <c r="F95" s="3">
+        <v>0</v>
+      </c>
+      <c r="G95" s="3">
         <v>109.8</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="3">
         <v>4.5</v>
       </c>
       <c r="I95" t="s">
@@ -3644,29 +3652,29 @@
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2014</v>
       </c>
       <c r="B96" t="s">
         <v>55</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="3">
         <v>3352</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="3">
         <v>40834</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="3">
         <v>11.5</v>
       </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-      <c r="G96">
+      <c r="F96" s="3">
+        <v>0</v>
+      </c>
+      <c r="G96" s="3">
         <v>112.8</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="3">
         <v>4.5</v>
       </c>
       <c r="I96" t="s">
@@ -3676,29 +3684,29 @@
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2015</v>
       </c>
       <c r="B97" t="s">
         <v>55</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="3">
         <v>3352</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="3">
         <v>40109</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="3">
         <v>11.5</v>
       </c>
-      <c r="F97">
-        <v>0</v>
-      </c>
-      <c r="G97">
+      <c r="F97" s="3">
+        <v>0</v>
+      </c>
+      <c r="G97" s="3">
         <v>115.4</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="3">
         <v>4.5</v>
       </c>
       <c r="I97" t="s">
@@ -3715,22 +3723,22 @@
       <c r="B98" t="s">
         <v>69</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="3">
         <v>190</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="3">
         <v>3790</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="3">
         <v>19</v>
       </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-      <c r="G98">
+      <c r="F98" s="3">
+        <v>0</v>
+      </c>
+      <c r="G98" s="3">
         <v>275.04000000000002</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="3">
         <v>6.1</v>
       </c>
       <c r="I98" t="s">
@@ -3747,22 +3755,22 @@
       <c r="B99" t="s">
         <v>69</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="3">
         <v>190</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="3">
         <v>3706</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="3">
         <v>19</v>
       </c>
-      <c r="F99">
-        <v>0</v>
-      </c>
-      <c r="G99">
+      <c r="F99" s="3">
+        <v>0</v>
+      </c>
+      <c r="G99" s="3">
         <v>281.89</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="3">
         <v>6.1</v>
       </c>
       <c r="I99" t="s">
@@ -3779,22 +3787,22 @@
       <c r="B100" t="s">
         <v>69</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="3">
         <v>190</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="3">
         <v>3625</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="3">
         <v>19</v>
       </c>
-      <c r="F100">
-        <v>0</v>
-      </c>
-      <c r="G100">
+      <c r="F100" s="3">
+        <v>0</v>
+      </c>
+      <c r="G100" s="3">
         <v>247.2</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="3">
         <v>6.1</v>
       </c>
       <c r="I100" t="s">
@@ -3811,22 +3819,22 @@
       <c r="B101" t="s">
         <v>69</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="3">
         <v>190</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="3">
         <v>3563</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="3">
         <v>19</v>
       </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
-      <c r="G101">
+      <c r="F101" s="3">
+        <v>0</v>
+      </c>
+      <c r="G101" s="3">
         <v>231.2</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="3">
         <v>6.1</v>
       </c>
       <c r="I101" t="s">
@@ -3843,22 +3851,22 @@
       <c r="B102" t="s">
         <v>69</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="3">
         <v>190</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="3">
         <v>3503</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="3">
         <v>19</v>
       </c>
-      <c r="F102">
-        <v>0</v>
-      </c>
-      <c r="G102">
+      <c r="F102" s="3">
+        <v>0</v>
+      </c>
+      <c r="G102" s="3">
         <v>235.1</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="3">
         <v>6.1</v>
       </c>
       <c r="I102" t="s">
@@ -3875,22 +3883,22 @@
       <c r="B103" t="s">
         <v>69</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="3">
         <v>190</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="3">
         <v>3393</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="3">
         <v>19</v>
       </c>
-      <c r="F103">
-        <v>0</v>
-      </c>
-      <c r="G103">
+      <c r="F103" s="3">
+        <v>0</v>
+      </c>
+      <c r="G103" s="3">
         <v>249</v>
       </c>
-      <c r="H103">
+      <c r="H103" s="3">
         <v>6.1</v>
       </c>
       <c r="I103" t="s">
@@ -3900,29 +3908,29 @@
         <v>59</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2010</v>
       </c>
       <c r="B104" t="s">
         <v>60</v>
       </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-      <c r="D104">
+      <c r="C104" s="3">
+        <v>0</v>
+      </c>
+      <c r="D104" s="3">
         <v>81277</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="3">
         <v>22.5</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="3">
         <v>1913</v>
       </c>
-      <c r="G104">
+      <c r="G104" s="3">
         <v>122.12</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="I104" t="s">
@@ -3932,29 +3940,29 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2011</v>
       </c>
       <c r="B105" t="s">
         <v>60</v>
       </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-      <c r="D105">
+      <c r="C105" s="3">
+        <v>0</v>
+      </c>
+      <c r="D105" s="3">
         <v>79469</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="3">
         <v>22.5</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="3">
         <v>2152</v>
       </c>
-      <c r="G105">
+      <c r="G105" s="3">
         <v>118.59</v>
       </c>
-      <c r="H105">
+      <c r="H105" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="I105" t="s">
@@ -3964,29 +3972,29 @@
         <v>62</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2012</v>
       </c>
       <c r="B106" t="s">
         <v>60</v>
       </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-      <c r="D106">
+      <c r="C106" s="3">
+        <v>0</v>
+      </c>
+      <c r="D106" s="3">
         <v>77785</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="3">
         <v>22.5</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="3">
         <v>2420</v>
       </c>
-      <c r="G106">
+      <c r="G106" s="3">
         <v>113</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="I106" t="s">
@@ -3996,29 +4004,29 @@
         <v>62</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2013</v>
       </c>
       <c r="B107" t="s">
         <v>60</v>
       </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
-      <c r="D107">
+      <c r="C107" s="3">
+        <v>0</v>
+      </c>
+      <c r="D107" s="3">
         <v>76227</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="3">
         <v>22.5</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="3">
         <v>2563</v>
       </c>
-      <c r="G107">
+      <c r="G107" s="3">
         <v>120.7</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="I107" t="s">
@@ -4028,29 +4036,29 @@
         <v>62</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2014</v>
       </c>
       <c r="B108" t="s">
         <v>60</v>
       </c>
-      <c r="C108">
-        <v>0</v>
-      </c>
-      <c r="D108">
+      <c r="C108" s="3">
+        <v>0</v>
+      </c>
+      <c r="D108" s="3">
         <v>74854</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="3">
         <v>22.5</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="3">
         <v>2632</v>
       </c>
-      <c r="G108">
+      <c r="G108" s="3">
         <v>121.2</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="I108" t="s">
@@ -4060,29 +4068,29 @@
         <v>62</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2015</v>
       </c>
       <c r="B109" t="s">
         <v>60</v>
       </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109">
+      <c r="C109" s="3">
+        <v>0</v>
+      </c>
+      <c r="D109" s="3">
         <v>73588</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="3">
         <v>22.5</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="3">
         <v>2676</v>
       </c>
-      <c r="G109">
+      <c r="G109" s="3">
         <v>117.6</v>
       </c>
-      <c r="H109">
+      <c r="H109" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="I109" t="s">
@@ -4092,29 +4100,29 @@
         <v>62</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2010</v>
       </c>
       <c r="B110" t="s">
         <v>63</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="3">
         <v>4661</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="3">
         <v>156527</v>
       </c>
-      <c r="E110">
+      <c r="E110" s="3">
         <v>30.5</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="3">
         <v>5026</v>
       </c>
-      <c r="G110">
+      <c r="G110" s="3">
         <v>86.42</v>
       </c>
-      <c r="H110">
+      <c r="H110" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="I110" t="s">
@@ -4124,29 +4132,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2011</v>
       </c>
       <c r="B111" t="s">
         <v>63</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="3">
         <v>4661</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="3">
         <v>156356</v>
       </c>
-      <c r="E111">
+      <c r="E111" s="3">
         <v>30.5</v>
       </c>
-      <c r="F111">
+      <c r="F111" s="3">
         <v>5628</v>
       </c>
-      <c r="G111">
+      <c r="G111" s="3">
         <v>83.53</v>
       </c>
-      <c r="H111">
+      <c r="H111" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="I111" t="s">
@@ -4156,29 +4164,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2012</v>
       </c>
       <c r="B112" t="s">
         <v>63</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="3">
         <v>4661</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="3">
         <v>156397</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="3">
         <v>30.5</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="3">
         <v>6150</v>
       </c>
-      <c r="G112">
+      <c r="G112" s="3">
         <v>81.400000000000006</v>
       </c>
-      <c r="H112">
+      <c r="H112" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="I112" t="s">
@@ -4188,29 +4196,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2013</v>
       </c>
       <c r="B113" t="s">
         <v>63</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="3">
         <v>4661</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="3">
         <v>156656</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="3">
         <v>30.5</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="3">
         <v>6864</v>
       </c>
-      <c r="G113">
+      <c r="G113" s="3">
         <v>79.8</v>
       </c>
-      <c r="H113">
+      <c r="H113" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="I113" t="s">
@@ -4220,29 +4228,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2014</v>
       </c>
       <c r="B114" t="s">
         <v>63</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="3">
         <v>4661</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="3">
         <v>157288</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="3">
         <v>30.5</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="3">
         <v>7471</v>
       </c>
-      <c r="G114">
+      <c r="G114" s="3">
         <v>77.599999999999994</v>
       </c>
-      <c r="H114">
+      <c r="H114" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="I114" t="s">
@@ -4252,29 +4260,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2015</v>
       </c>
       <c r="B115" t="s">
         <v>63</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="3">
         <v>4661</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="3">
         <v>158196</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="3">
         <v>30.5</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="3">
         <v>7194</v>
       </c>
-      <c r="G115">
+      <c r="G115" s="3">
         <v>73.5</v>
       </c>
-      <c r="H115">
+      <c r="H115" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="I115" t="s">
@@ -4284,29 +4292,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2010</v>
       </c>
       <c r="B116" t="s">
         <v>66</v>
       </c>
-      <c r="C116">
-        <v>0</v>
-      </c>
-      <c r="D116">
+      <c r="C116" s="3">
+        <v>0</v>
+      </c>
+      <c r="D116" s="3">
         <v>1625</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="3">
         <v>16.289473684210531</v>
       </c>
-      <c r="F116">
-        <v>0</v>
-      </c>
-      <c r="G116">
+      <c r="F116" s="3">
+        <v>0</v>
+      </c>
+      <c r="G116" s="3">
         <v>74.459999999999994</v>
       </c>
-      <c r="H116">
+      <c r="H116" s="3">
         <v>4.3473684210526322</v>
       </c>
       <c r="I116" t="s">
@@ -4316,29 +4324,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2011</v>
       </c>
       <c r="B117" t="s">
         <v>66</v>
       </c>
-      <c r="C117">
-        <v>0</v>
-      </c>
-      <c r="D117">
+      <c r="C117" s="3">
+        <v>0</v>
+      </c>
+      <c r="D117" s="3">
         <v>1588</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="3">
         <v>16.289473684210531</v>
       </c>
-      <c r="F117">
-        <v>0</v>
-      </c>
-      <c r="G117">
+      <c r="F117" s="3">
+        <v>0</v>
+      </c>
+      <c r="G117" s="3">
         <v>72.8</v>
       </c>
-      <c r="H117">
+      <c r="H117" s="3">
         <v>4.3473684210526322</v>
       </c>
       <c r="I117" t="s">
@@ -4348,29 +4356,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2012</v>
       </c>
       <c r="B118" t="s">
         <v>66</v>
       </c>
-      <c r="C118">
-        <v>0</v>
-      </c>
-      <c r="D118">
+      <c r="C118" s="3">
+        <v>0</v>
+      </c>
+      <c r="D118" s="3">
         <v>1560</v>
       </c>
-      <c r="E118">
+      <c r="E118" s="3">
         <v>16.289473684210531</v>
       </c>
-      <c r="F118">
-        <v>0</v>
-      </c>
-      <c r="G118">
+      <c r="F118" s="3">
+        <v>0</v>
+      </c>
+      <c r="G118" s="3">
         <v>61.3</v>
       </c>
-      <c r="H118">
+      <c r="H118" s="3">
         <v>4.3473684210526322</v>
       </c>
       <c r="I118" t="s">
@@ -4380,29 +4388,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2013</v>
       </c>
       <c r="B119" t="s">
         <v>66</v>
       </c>
-      <c r="C119">
-        <v>0</v>
-      </c>
-      <c r="D119">
+      <c r="C119" s="3">
+        <v>0</v>
+      </c>
+      <c r="D119" s="3">
         <v>1541</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="3">
         <v>16.289473684210531</v>
       </c>
-      <c r="F119">
-        <v>0</v>
-      </c>
-      <c r="G119">
+      <c r="F119" s="3">
+        <v>0</v>
+      </c>
+      <c r="G119" s="3">
         <v>53.4</v>
       </c>
-      <c r="H119">
+      <c r="H119" s="3">
         <v>4.3473684210526322</v>
       </c>
       <c r="I119" t="s">
@@ -4412,29 +4420,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2014</v>
       </c>
       <c r="B120" t="s">
         <v>66</v>
       </c>
-      <c r="C120">
-        <v>0</v>
-      </c>
-      <c r="D120">
+      <c r="C120" s="3">
+        <v>0</v>
+      </c>
+      <c r="D120" s="3">
         <v>1537</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="3">
         <v>16.289473684210531</v>
       </c>
-      <c r="F120">
-        <v>0</v>
-      </c>
-      <c r="G120">
+      <c r="F120" s="3">
+        <v>0</v>
+      </c>
+      <c r="G120" s="3">
         <v>55.5</v>
       </c>
-      <c r="H120">
+      <c r="H120" s="3">
         <v>4.3473684210526322</v>
       </c>
       <c r="I120" t="s">
@@ -4444,29 +4452,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2015</v>
       </c>
       <c r="B121" t="s">
         <v>66</v>
       </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-      <c r="D121">
+      <c r="C121" s="3">
+        <v>0</v>
+      </c>
+      <c r="D121" s="3">
         <v>1539</v>
       </c>
-      <c r="E121">
+      <c r="E121" s="3">
         <v>16.289473684210531</v>
       </c>
-      <c r="F121">
-        <v>0</v>
-      </c>
-      <c r="G121">
+      <c r="F121" s="3">
+        <v>0</v>
+      </c>
+      <c r="G121" s="3">
         <v>52</v>
       </c>
-      <c r="H121">
+      <c r="H121" s="3">
         <v>4.3473684210526322</v>
       </c>
       <c r="I121" t="s">
@@ -4477,13 +4485,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J121" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="la Candelaria"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J121" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>